<commit_message>
add stage 1 evidence
</commit_message>
<xml_diff>
--- a/si35/evidence.xlsx
+++ b/si35/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="56">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -130,12 +130,30 @@
     <t xml:space="preserve">class id you issued</t>
   </si>
   <si>
+    <t xml:space="preserve">DA3C32FEE00C1B908BACFCF7736A061D2E01A93A435C44D80F7BF5E3E6138E71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35collection2</t>
+  </si>
+  <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
     <t xml:space="preserve">nft id you minted</t>
   </si>
   <si>
+    <t xml:space="preserve">C0E937E3A34811038B8BE38A41D29DFEF1AC51F3C2DED735EA546800AD92DA43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35nft3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3F4E822559E89021E94690F5E73D5C767AAAC233D8E33920C7E51891A1A01763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35nft4</t>
+  </si>
+  <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
@@ -148,10 +166,37 @@
     <t xml:space="preserve">dest chain id</t>
   </si>
   <si>
+    <t xml:space="preserve">F8D29FFDD20A0D89B2FCA8CF8547EF1878CBA76331755718FF028F90B3024C48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/si35collection2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elgafar-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8E1BAFD0771B5BEDF7F85AB94ED33FF9799A240F6319E37512BDF0A581E3D895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/395E24580861A7A0444F0A5155F9FC18110BDC6D163E043DF8FE95ADF6AB0F97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-flixnet-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">tx hash on dest chain</t>
   </si>
   <si>
     <t xml:space="preserve">ibc class on chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAB039418601CE4A54EF2308F74EB2405040348E9B7BBDFB562C0AF4481FB370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stars185uarznjds070syl8ydfgvmque7rxzxceehlt75zfw4v0e7dq0rsnujkhl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0E87E590BEDEDBD0D5E52C19D8DC1C9BBCC433C0BA5ED5128FCB2EAE69BE97C8</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -376,11 +421,11 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -491,7 +536,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -501,15 +546,15 @@
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -534,7 +579,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -544,15 +589,15 @@
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +622,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -587,15 +632,15 @@
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -620,7 +665,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -630,15 +675,15 @@
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -663,7 +708,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -673,25 +718,25 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +761,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -726,25 +771,25 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +814,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -779,25 +824,25 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +867,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -832,25 +877,25 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -875,7 +920,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -885,25 +930,25 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -928,7 +973,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -938,25 +983,25 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -975,15 +1020,66 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,68 +1087,25 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1077,7 +1130,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1087,25 +1140,25 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1130,7 +1183,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1139,12 +1192,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1169,7 +1222,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1178,12 +1231,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1208,7 +1261,7 @@
       <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1217,12 +1270,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1247,7 +1300,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1256,12 +1309,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1280,13 +1333,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1300,7 +1353,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,8 +1364,30 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1330,13 +1405,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1350,10 +1425,10 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,14 +1436,28 @@
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1386,13 +1475,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1406,10 +1495,10 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,13 +1506,27 @@
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1442,13 +1545,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1462,25 +1565,39 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1498,13 +1615,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
@@ -1520,38 +1637,95 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1562,7 +1736,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1572,58 +1746,15 @@
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add stage 2 evidence
</commit_message>
<xml_diff>
--- a/si35/evidence.xlsx
+++ b/si35/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -148,19 +148,157 @@
     <t xml:space="preserve">0E87E590BEDEDBD0D5E52C19D8DC1C9BBCC433C0BA5ED5128FCB2EAE69BE97C8</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on that chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on that chain	chain id</t>
+    <t xml:space="preserve">ibc/88D48D2EE86214DAB6EC92B1CD3DB16A783B3150C725859A9F19EB22EBCF822D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35nft5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/EC2B8D84C5F5A0095DCF45993536AE9CF0CCA87F184E57DAFA5CA0C95A7560A5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35nft6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/CD72370D713C37CA39449CE36B25A67C2FBEDF9C8C7ACEA1D2D9B758F4811B69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35nft7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/D556E52A2E6FA74F28836823BCFD339573B2F7F475BFE5D3E5ADFDC217B6A881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35nft8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/8BD3FBEF2823F89DF3F02146AD8BB0BADA1832E389F9414FA7B352135E83728E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35nft9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/78F638631E2DF9CC1767809B789205F7550E73E5B777A7B3E9D0AD4225BE3078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si35nft10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7B4948957F08306C0547D3164E80BB018AE206D178DC89171F62706C59FABE4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-irishub-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86CFF06B297CE6156B99C010E5600CF7659A6F19F271632D4E50075748404DB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158BAAE311FDE210A554AEA94C4858E9E9AB03C4F71080ECC12F5025C0CAEEDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uptick_7000-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41ED6962A35E73545DADD91CB8ADC044A9582324D657E03204AED2E5A2FE9250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E34A36E9BE8927CF1785E07F080FC8D7D4A81C8A9EBC09220F73026D913781E4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F380E99C459876E2CFA240346125EBA62792307167B2C4AAA177BF0E0866708B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE6E170C1BEC6EC825D08DCE202C8A74ACE140411878448DF80E9E9F88905CDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3C598587CD56655D80F1891FF5F5F85EE9B0F853DFC285844801CED70DAD1A5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C906F2959789DBB802798D863C1ABF232803080ED3A2C2899CC5E6008DED8865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1A45184520F86C47A5F30A32487734952439E26770D60EDD8908E78FBD31355D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uni-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F918707EA09AB000FE96AAD115228F19838532CD6941FF2C5993682AAF49F96B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9768A3DCC013AC0C8269282BE48E516861FFDDC595B3A0432153F9E827C4FB2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7915CBE33AC9E8CACB73B9A06CCEBAF0EBB3EE606B3231868E750CD1A36070D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7A54059E7A89E45F0007AD44EDE5AD3FEE34A975712372C56D739B078A62757C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">452254DE4CA8A37A31F8F556BA7B61A849FDC7B31CD554450BC1039A46F66A51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12676CE4F919EC70C08E402C5A9A4E5E33FF208446DA54390043A12F4FAC7901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBC9A3C0871C84C9CFE0387F756140FB29618305DAA1C44F02465517B3AE5492</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43C3C964ACABCD2414BE63E93F55037F049690426CFB68CC479EEA8C1C9CF2BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0F87201B487C2B8AAFF4F9804505FDF7F89FEC82BCFD3CD82145D61C83C2AE1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10D526C2EB31CD191B6612D778327445A692000A4287BEF3F1D27226C5EB346A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8C4E9AA9D315B1846FD9901AC23756122B819006A0D8653BD63954B9B8E4DDF5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC6184413F88E321B959FD4D7D732BD9981E658A6B187D2067C8DA75BA56BBBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFB9337E3B957377C124ECBC1340374570D6234E91A8EFD06273BDE149718AF1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94B05DAADA98C090B21D04F6CB1917622FE463B32CC05047B8D7A1D4C5F2B218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">305049C5EE2890E72F403A7B339E464C732F9CF2BF65E4427A3516F51A72B4CF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37F7C2D9EA02D2033CFF9D15BC1437980FF49CFCE3DD608E5967D0EAB578E30E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8DFB377087E0FF6DBCC44289D6EF5DA5285E5AD9854D76BC900382A6B222117A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1B0F543C6E8E190244892F4712261BC2E297A8870F3BFFCD8BD5F123A62BF4D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7808726F12A0E91054732E4DACCA68805A759956C6072EE359445D7FC0752FBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5E19DB60F234ED577909EA1C35F7E91112E1B4EF4C611947CEE3866EA4BB062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">380297607D836C6D2D39BAAAB2F3689D3A1A2F1D45A9F60A637A7AFD722E582F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B74FF52AD4A9D37934958DE4273B3E55A5B0D8BFF951E520F53CF2BE9C4E5D7A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">117AD10C0B4C35FE1AA41FA4585CD9E6966CA63B733B7E1175CF9FB14D2CA98B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">515A70E915444E626D629C9497E7443D7E60615B6FCBFB7F3A813571C899EEFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0F543B4ED58EDC277667B0D3D44109FDEA199F2404CC7F1A76293EC9D7BC62E2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4747A64C69036079DC27D2E7E09B8248EA6F8D600CDB3F32C823FA3F23017AE0</t>
   </si>
   <si>
     <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
@@ -268,7 +406,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,11 +419,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,7 +518,7 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -458,10 +600,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -476,10 +618,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -501,10 +643,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -519,10 +661,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -544,10 +686,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -562,10 +704,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -587,10 +729,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -605,10 +747,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -627,13 +769,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -648,20 +790,34 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -680,13 +836,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -701,20 +857,34 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -733,13 +903,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -752,22 +922,36 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -786,13 +970,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -805,22 +989,36 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>63</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -839,13 +1037,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -858,22 +1056,36 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>67</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -892,13 +1104,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -911,22 +1123,36 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>71</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -951,7 +1177,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
   </cols>
@@ -988,108 +1214,246 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
-  </cols>
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
+      <c r="A2" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1097,24 +1461,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>39</v>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1128,7 +1492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1136,10 +1500,10 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1147,13 +1511,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>39</v>
+      <c r="A2" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1167,84 +1531,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1256,7 +1542,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1317,7 +1603,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1373,7 +1659,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1429,7 +1715,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1481,11 +1767,11 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
@@ -1540,10 +1826,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1583,10 +1869,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1601,10 +1887,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add stage 3 evidence
</commit_message>
<xml_diff>
--- a/si35/evidence.xlsx
+++ b/si35/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -299,6 +299,18 @@
   </si>
   <si>
     <t xml:space="preserve">4747A64C69036079DC27D2E7E09B8248EA6F8D600CDB3F32C823FA3F23017AE0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67412629C7A405512E1A276D60505ACE216DE5BFFCD4468291FD0820252D523B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2F624EA99393BC7509192631798273BE5414BE77C5063269FCF735D098E7880F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">080DBC64CC77863C44C56967522179A42200745892244AA5C5E3AEC0F4F6AB6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEC88DA2A370D7DE244D706EBB9A2ED7B6842AEA94649FAF9FF5D77016A1E05A</t>
   </si>
   <si>
     <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
@@ -314,7 +326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -343,12 +355,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -406,7 +412,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -427,11 +433,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,7 +520,7 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -603,7 +605,7 @@
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -646,7 +648,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -689,7 +691,7 @@
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -732,7 +734,7 @@
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -775,7 +777,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -842,7 +844,7 @@
       <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -909,7 +911,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -976,7 +978,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1001,7 +1003,7 @@
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1009,7 +1011,7 @@
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1017,7 +1019,7 @@
       <c r="A5" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1043,7 +1045,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1068,7 +1070,7 @@
       <c r="A3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1076,7 +1078,7 @@
       <c r="A4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1084,7 +1086,7 @@
       <c r="A5" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1110,7 +1112,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1177,7 +1179,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
   </cols>
@@ -1220,7 +1222,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1245,7 +1247,7 @@
       <c r="A3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1253,7 +1255,7 @@
       <c r="A4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1261,7 +1263,7 @@
       <c r="A5" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1269,7 +1271,7 @@
       <c r="A6" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1277,7 +1279,7 @@
       <c r="A7" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1299,11 +1301,11 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1328,7 +1330,7 @@
       <c r="A3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1336,7 +1338,7 @@
       <c r="A4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1344,7 +1346,7 @@
       <c r="A5" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1352,7 +1354,7 @@
       <c r="A6" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1360,7 +1362,7 @@
       <c r="A7" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1383,10 +1385,10 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1394,13 +1396,91 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1422,10 +1502,10 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1433,13 +1513,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>85</v>
+      <c r="A2" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1453,84 +1533,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1542,7 +1544,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1603,7 +1605,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1659,7 +1661,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1715,7 +1717,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1771,7 +1773,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
@@ -1829,7 +1831,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1872,7 +1874,7 @@
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>

</xml_diff>

<commit_message>
Update stage 3 evidence - B5, B6, B7
</commit_message>
<xml_diff>
--- a/si35/evidence.xlsx
+++ b/si35/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
     <sheet name="B2" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="B5" sheetId="24" state="visible" r:id="rId25"/>
     <sheet name="B6" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="B7" sheetId="26" state="visible" r:id="rId27"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -313,10 +314,22 @@
     <t xml:space="preserve">FEC88DA2A370D7DE244D706EBB9A2ED7B6842AEA94649FAF9FF5D77016A1E05A</t>
   </si>
   <si>
-    <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Internal Transfer TxHash on IRISnet</t>
+    <t xml:space="preserve">5B1BAC940DFAA64F89C06FE015255763005BC9A05DEC37BB17ACE3DEF4362AD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56126EE58C0DB25C0CABDC51AA7731C1F013621EB9D574ED4108D20F2AA77A0D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B4C3981F3179E5C497F2F32DDCAE135701936304C3AB4E88B7482761D9646EB5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C59F06A0F66BF6ED9AC460B5828913B6DB7BA073C3D0C05359FE6CCBF76FA0AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">484F33128ABDA933E0E0D1A7238BB5455D34946B82F2069741A6CD4C365EB886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2C53F0C123AB41AA34D96CB0C78FA3673A90DE1000E64ADC0B3D3223CDF7A701</t>
   </si>
 </sst>
 </file>
@@ -520,7 +533,7 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -605,7 +618,7 @@
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -648,7 +661,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -691,7 +704,7 @@
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -734,7 +747,7 @@
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -777,7 +790,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -844,7 +857,7 @@
       <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -911,7 +924,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -978,7 +991,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1045,7 +1058,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1112,7 +1125,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1179,7 +1192,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
   </cols>
@@ -1222,7 +1235,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1305,7 +1318,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1388,7 +1401,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1423,11 +1436,11 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1463,22 +1476,22 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>90</v>
       </c>
@@ -1502,24 +1515,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1533,6 +1546,45 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1544,7 +1596,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1605,7 +1657,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1661,7 +1713,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1717,7 +1769,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1773,7 +1825,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
@@ -1831,7 +1883,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1874,7 +1926,7 @@
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>

</xml_diff>